<commit_message>
Reajuste de mapeado, V1 (Basic)
</commit_message>
<xml_diff>
--- a/SW/Arduino/V1/GPIO_Teclado_Macros_V1.xlsx
+++ b/SW/Arduino/V1/GPIO_Teclado_Macros_V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositorios\Proyectos Finalizados\Teclado-Macros-BT-ESP32\SW\Arduino\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\Proyectos 2024\Teclado-Macros-BT-ESP32\SW\Arduino\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A774B0E-B465-4E34-B4EB-066D62EF57ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E491BA-F51B-4074-99EF-892731C38F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="4440" windowWidth="20640" windowHeight="11040" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{1CC31A59-071C-4B79-B480-A3CD3D0586A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
     <t>Shift+win+s</t>
   </si>
   <si>
-    <t>win+l</t>
+    <t>win+k</t>
   </si>
 </sst>
 </file>
@@ -796,21 +796,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D00BFD8-8064-4ED2-A3E0-704A30F9AE96}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="11.42578125" style="4"/>
-    <col min="7" max="7" width="13.5703125" style="4" customWidth="1"/>
-    <col min="8" max="10" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="6" width="11.44140625" style="4"/>
+    <col min="7" max="7" width="13.5546875" style="4" customWidth="1"/>
+    <col min="8" max="10" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -819,7 +819,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -862,7 +862,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -891,7 +891,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -920,7 +920,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -934,7 +934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -993,7 +993,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>11</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>12</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>13</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>14</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>15</v>
       </c>

</xml_diff>